<commit_message>
schedule_mate clashing tasks, hours, max duration
</commit_message>
<xml_diff>
--- a/schedule_mate/schedule_mate_output.xlsx
+++ b/schedule_mate/schedule_mate_output.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +450,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>start_date</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>end</t>
+          <t>end_date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>duration</t>
+          <t>time(h)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -478,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pénzügyek tanóra</t>
+          <t>Tanulni Makroökonómia vizsgára</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,51 +490,47 @@
           <t>Iskola</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-03-17 09:00</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-03-17 13:00</t>
-        </is>
+      <c r="C2" s="2" t="n">
+        <v>45733.35416666666</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45733.375</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+        <v>1.5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kerékpározás</t>
+          <t>Pénzügyek tanóra</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Regeneráció</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-03-17 13:30</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-03-17 15:00</t>
-        </is>
+          <t>Iskola</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45733.375</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45733.54166666666</v>
       </c>
       <c r="E3" t="n">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
@@ -538,37 +538,37 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Baráti kocsmázás</t>
+          <t>Tanulni Makroökonómia vizsgára</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Szociális</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-03-17 15:30</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-03-17 19:30</t>
-        </is>
+          <t>Iskola</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45733.54166666666</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45733.5625</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+        <v>1.5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jóga</t>
+          <t>Kerékpározás</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -576,21 +576,17 @@
           <t>Regeneráció</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-03-17 20:00</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-03-17 21:00</t>
-        </is>
+      <c r="C5" s="2" t="n">
+        <v>45733.5625</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45733.625</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
@@ -598,269 +594,619 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Data analysis webinár</t>
+          <t>Tanulni Makroökonómia vizsgára</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hosszú távú célok</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-03-17 21:10</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-03-17 22:40</t>
-        </is>
+          <t>Iskola</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45733.625</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45733.64583333334</v>
       </c>
       <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
         <v>1.5</v>
       </c>
-      <c r="F6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tanulni Makroökonómia vizsgára</t>
+          <t>Baráti kocsmázás</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Iskola</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-03-18 08:30</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-03-18 10:00</t>
-        </is>
+          <t>Szociális</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45733.64583333334</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45733.8125</v>
       </c>
       <c r="E7" t="n">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>10</v>
-      </c>
-      <c r="H7" t="n">
-        <v>9</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nyújtás</t>
+          <t>Tanulni Makroökonómia vizsgára</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Regeneráció</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-03-18 10:00</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-03-18 11:15</t>
-        </is>
+          <t>Iskola</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45733.8125</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45733.83333333334</v>
       </c>
       <c r="E8" t="n">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="F8" t="n">
-        <v>0.625</v>
+        <v>1.5</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H8" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Családi találkozó</t>
+          <t>Jóga</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Szociális</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-03-18 11:15</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2025-03-18 15:15</t>
-        </is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45733.83333333334</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45733.875</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" t="n">
-        <v>6</v>
-      </c>
-      <c r="H9" t="n">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pihenés</t>
+          <t>Data analysis webinár</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Regeneráció</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-03-18 15:15</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>2025-03-18 15:52</t>
-        </is>
+          <t>Hosszú távú célok</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45733.88194444445</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45733.94444444445</v>
       </c>
       <c r="E10" t="n">
-        <v>0.625</v>
+        <v>1.5</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3125</v>
-      </c>
-      <c r="G10" t="n">
-        <v>5</v>
-      </c>
-      <c r="H10" t="n">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Data analysis tanulása</t>
+          <t>Tanulni Makroökonómia vizsgára</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hosszú távú célok</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-03-18 15:52</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2025-03-18 18:22</t>
-        </is>
+          <t>Iskola</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45734.35416666666</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45734.45833333334</v>
       </c>
       <c r="E11" t="n">
         <v>2.5</v>
       </c>
       <c r="F11" t="n">
-        <v>3.75</v>
+        <v>7.5</v>
       </c>
       <c r="G11" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Olvasás</t>
+          <t>Data analysis tanulása</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Szokások, heti célok</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2025-03-18 18:22</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2025-03-18 19:02</t>
-        </is>
+          <t>Hosszú távú célok</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45734.45833333334</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45734.5625</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6666666666666666</v>
+        <v>2.5</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8333333333333333</v>
+        <v>3.75</v>
       </c>
       <c r="G12" t="n">
         <v>7</v>
       </c>
       <c r="H12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Családi találkozó</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Szociális</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45734.5625</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45734.77083333334</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Olvasás</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Szokások, heti célok</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45734.77083333334</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45734.8125</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G14" t="n">
+        <v>7</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Nyújtás</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45734.8125</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45734.875</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pihenés</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45734.875</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45734.91666666666</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Data analysis tanulása</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Hosszú távú célok</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45735.35416666666</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45735.45833333334</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7</v>
+      </c>
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Olvasás</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Szokások, heti célok</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45735.45833333334</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45735.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Nyújtás</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45735.5</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45735.5625</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G19" t="n">
+        <v>6</v>
+      </c>
+      <c r="H19" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Pihenés</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45735.5625</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45735.60416666666</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>Ötletelés chatgpt-vel</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>Egyéb</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2025-03-18 19:02</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>2025-03-18 20:02</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
+      <c r="C21" s="2" t="n">
+        <v>45735.60416666666</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45735.66666666666</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3</v>
+      </c>
+      <c r="H21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Data analysis tanulása</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Hosszú távú célok</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45736.35416666666</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>45736.45833333334</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F22" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7</v>
+      </c>
+      <c r="H22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Olvasás</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Szokások, heti célok</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45736.45833333334</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>45736.5</v>
+      </c>
+      <c r="E23" t="n">
         <v>1</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F23" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7</v>
+      </c>
+      <c r="H23" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Nyújtás</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45736.5</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>45736.5625</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Pihenés</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45736.5625</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>45736.60416666666</v>
+      </c>
+      <c r="E25" t="n">
         <v>1</v>
       </c>
-      <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="n">
-        <v>4</v>
+      <c r="F25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Pihenés</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Regeneráció</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>45737.35416666666</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>45737.39583333334</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>